<commit_message>
Fixing mappings towards IOTDB for export
</commit_message>
<xml_diff>
--- a/test/sample_forms/Form-4SF-update.xlsx
+++ b/test/sample_forms/Form-4SF-update.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\base\forms\base-form-management\test\sample_forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FBD204-F45F-4AC4-A2E8-9A1D162EB0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4487457-D137-437D-B6AF-7E1306BEE241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="jbPe6SBLf4oG4Cgxdp2GTHPCnTakxOLusQvs3FLR97ZGw7ZrHwFP80gs+fK1zVtwmXmlsYM45w/LTktaEDAlHA==" workbookSaltValue="+e6btQraNKSRCi9yKssXHA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1527,7 +1527,7 @@
   <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,7 +2030,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6:H433"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>